<commit_message>
exam time table also created
</commit_message>
<xml_diff>
--- a/plannerAgentBackend/uploaded_exams/planner_agent_data_nushan.xlsx
+++ b/plannerAgentBackend/uploaded_exams/planner_agent_data_nushan.xlsx
@@ -18,12 +18,14 @@
     <sheet name="Semester 4" sheetId="4" r:id="rId4"/>
     <sheet name="Semester 5" sheetId="5" r:id="rId5"/>
     <sheet name="module codes" sheetId="6" r:id="rId6"/>
-    <sheet name="Sheet6" sheetId="13" r:id="rId7"/>
-    <sheet name="Sheet5" sheetId="12" r:id="rId8"/>
-    <sheet name="module codes2" sheetId="8" r:id="rId9"/>
-    <sheet name="Sheet2" sheetId="10" r:id="rId10"/>
-    <sheet name="Sheet4" sheetId="11" r:id="rId11"/>
-    <sheet name="halls" sheetId="7" r:id="rId12"/>
+    <sheet name="Sheet1" sheetId="14" r:id="rId7"/>
+    <sheet name="Sheet6" sheetId="13" r:id="rId8"/>
+    <sheet name="Sheet5" sheetId="12" r:id="rId9"/>
+    <sheet name="module codes2" sheetId="8" r:id="rId10"/>
+    <sheet name="Sheet2" sheetId="10" r:id="rId11"/>
+    <sheet name="Sheet4" sheetId="11" r:id="rId12"/>
+    <sheet name="halls" sheetId="7" r:id="rId13"/>
+    <sheet name="halls-exam" sheetId="15" r:id="rId14"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7801" uniqueCount="1323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7973" uniqueCount="1425">
   <si>
     <t>Hall</t>
   </si>
@@ -4004,6 +4006,312 @@
   </si>
   <si>
     <t>IS8201: Day=Sun, Hall=AUD, Slot=4</t>
+  </si>
+  <si>
+    <t>CE1202: Day=Fri2, Slot=0, Hall=AUD, Students=550, Dept=CE</t>
+  </si>
+  <si>
+    <t>CE1101: Day=Thu2, Slot=0, Hall=AUD, Students=550, Dept=CE</t>
+  </si>
+  <si>
+    <t>EE1301: Day=Sat2, Slot=1, Hall=AUD, Students=550, Dept=EE</t>
+  </si>
+  <si>
+    <t>EE1101: Day=Sat2, Slot=0, Hall=AUD, Students=550, Dept=EE</t>
+  </si>
+  <si>
+    <t>ME1201: Day=Thu, Slot=0, Hall=AUD, Students=550, Dept=ME</t>
+  </si>
+  <si>
+    <t>ME1202: Day=Sun2, Slot=0, Hall=AUD, Students=550, Dept=ME</t>
+  </si>
+  <si>
+    <t>IS1402: Day=Fri2, Slot=1, Hall=AUD, Students=550, Dept=IS</t>
+  </si>
+  <si>
+    <t>IS1301: Day=Wed, Slot=0, Hall=AUD, Students=550, Dept=IS</t>
+  </si>
+  <si>
+    <t>IS1003: Day=Tue, Slot=1, Hall=AUD, Students=550, Dept=IS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CE3201: Day=Tue2, Slot=1, Hall=Civil-COBEU, Students=100, Dept=CE  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CE3202: Day=Thu, Slot=0, Hall=Civil-COBEU, Students=100, Dept=CE   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CE3303: Day=Tue2, Slot=0, Hall=Civil-COBEU, Students=100, Dept=CE  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CE3304: Day=Mon2, Slot=1, Hall=Civil-COBEU, Students=100, Dept=CE  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CE3205: Day=Sat2, Slot=0, Hall=Civil-COBEU, Students=100, Dept=CE  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EE3301: Day=Mon, Slot=0, Hall=Civil-CSR, Students=75, Dept=EE      </t>
+  </si>
+  <si>
+    <t>EE3202: Day=Mon2, Slot=0, Hall=LR1, Students=75, Dept=EE</t>
+  </si>
+  <si>
+    <t>EE3203: Day=Wed2, Slot=1, Hall=LT1, Students=75, Dept=EE</t>
+  </si>
+  <si>
+    <t>EE3304: Day=Thu, Slot=1, Hall=DO2, Students=75, Dept=EE</t>
+  </si>
+  <si>
+    <t>EE3205: Day=Mon2, Slot=1, Hall=Electrical-ESR, Students=75, Dept=EE</t>
+  </si>
+  <si>
+    <t>EE3306: Day=Fri, Slot=1, Hall=I.S. Seminar Room, Students=75, Dept=EE</t>
+  </si>
+  <si>
+    <t>EC3301: Day=Wed, Slot=1, Hall=New Computer Center, Students=200, Dept=EC</t>
+  </si>
+  <si>
+    <t>EC3202: Day=Fri2, Slot=1, Hall=LT1, Students=200, Dept=EC</t>
+  </si>
+  <si>
+    <t>EC3203: Day=Fri, Slot=0, Hall=LT1, Students=200, Dept=EC</t>
+  </si>
+  <si>
+    <t>EC3404: Day=Wed2, Slot=1, Hall=New Computer Center, Students=200, Dept=EC</t>
+  </si>
+  <si>
+    <t>EC3305: Day=Sat2, Slot=1, Hall=New Computer Center, Students=200, Dept=EC</t>
+  </si>
+  <si>
+    <t>ME3301: Day=Wed2, Slot=0, Hall=LT2, Students=75, Dept=ME</t>
+  </si>
+  <si>
+    <t>ME3202: Day=Sat2, Slot=0, Hall=Electrical-ECC, Students=75, Dept=ME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ME3303: Day=Sat, Slot=0, Hall=Electrical-ESR, Students=75, Dept=ME </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ME3204: Day=Wed, Slot=0, Hall=Electrical-ECC, Students=75, Dept=ME </t>
+  </si>
+  <si>
+    <t>ME3305: Day=Thu, Slot=1, Hall=NLH3, Students=75, Dept=ME</t>
+  </si>
+  <si>
+    <t>ME3206: Day=Tue, Slot=0, Hall=LR1, Students=75, Dept=ME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ME3210: Day=Mon, Slot=1, Hall=Electrical-ECC, Students=75, Dept=ME </t>
+  </si>
+  <si>
+    <t>IS3321: Day=Wed2, Slot=0, Hall=AUD, Students=550, Dept=IS</t>
+  </si>
+  <si>
+    <t>IS3301: Day=Wed, Slot=1, Hall=AUD, Students=550, Dept=IS</t>
+  </si>
+  <si>
+    <t>IS3322: Day=Sat, Slot=0, Hall=AUD, Students=550, Dept=IS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CE5301: Day=Wed, Slot=1, Hall=Civil-COBEU, Students=100, Dept=CE   </t>
+  </si>
+  <si>
+    <t>CE5202: Day=Fri, Slot=1, Hall=LR1, Students=100, Dept=CE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CE5303: Day=Tue, Slot=1, Hall=Civil-COBEU, Students=100, Dept=CE   </t>
+  </si>
+  <si>
+    <t>CE5204: Day=Mon2, Slot=0, Hall=DO1, Students=100, Dept=CE</t>
+  </si>
+  <si>
+    <t>CE5205: Day=Sun2, Slot=1, Hall=LR2, Students=100, Dept=CE</t>
+  </si>
+  <si>
+    <t>CE5306: Day=Sun, Slot=0, Hall=LR2, Students=100, Dept=CE</t>
+  </si>
+  <si>
+    <t>CE5251: Day=Thu2, Slot=1, Hall=LT1, Students=100, Dept=CE</t>
+  </si>
+  <si>
+    <t>CE5252: Day=Sun2, Slot=0, Hall=I.S. Seminar Room, Students=100, Dept=CE</t>
+  </si>
+  <si>
+    <t>EE5201: Day=Thu2, Slot=1, Hall=Electrical-ECC, Students=75, Dept=EE</t>
+  </si>
+  <si>
+    <t>EE5302: Day=Sat2, Slot=0, Hall=Electrical-ESR, Students=75, Dept=EE</t>
+  </si>
+  <si>
+    <t>EE5303: Day=Tue2, Slot=1, Hall=New Computer Center, Students=75, Dept=EE</t>
+  </si>
+  <si>
+    <t>EE5304: Day=Mon, Slot=1, Hall=DO2, Students=75, Dept=EE</t>
+  </si>
+  <si>
+    <t>EE5305: Day=Sun2, Slot=1, Hall=DO2, Students=75, Dept=EE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EE5206: Day=Fri, Slot=0, Hall=Electrical-ECC, Students=75, Dept=EE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EE5207: Day=Tue2, Slot=0, Hall=Civil-CSR, Students=75, Dept=EE     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EE5208: Day=Sun, Slot=0, Hall=Civil-COBEU, Students=75, Dept=EE    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EE5209: Day=Wed, Slot=0, Hall=Electrical-ESR, Students=75, Dept=EE </t>
+  </si>
+  <si>
+    <t>EE5453: Day=Fri2, Slot=0, Hall=LT2, Students=200, Dept=EE</t>
+  </si>
+  <si>
+    <t>EE5250: Day=Fri, Slot=0, Hall=LT2, Students=200, Dept=EE</t>
+  </si>
+  <si>
+    <t>EE5351: Day=Tue, Slot=0, Hall=LT1, Students=200, Dept=EE</t>
+  </si>
+  <si>
+    <t>EE5253: Day=Thu, Slot=0, Hall=New Computer Center, Students=200, Dept=EE</t>
+  </si>
+  <si>
+    <t>EE5454: Day=Thu2, Slot=0, Hall=New Computer Center, Students=200, Dept=EE</t>
+  </si>
+  <si>
+    <t>IS5311: Day=Thu, Slot=1, Hall=AUD, Students=550, Dept=IS</t>
+  </si>
+  <si>
+    <t>EE5260: Day=Sat, Slot=0, Hall=LT2, Students=200, Dept=EE</t>
+  </si>
+  <si>
+    <t>EE5261: Day=Fri2, Slot=1, Hall=New Computer Center, Students=200, Dept=EE</t>
+  </si>
+  <si>
+    <t>EE5262: Day=Wed2, Slot=0, Hall=LT1, Students=200, Dept=EE</t>
+  </si>
+  <si>
+    <t>ME5301: Day=Sun, Slot=0, Hall=LT2, Students=75, Dept=ME</t>
+  </si>
+  <si>
+    <t>ME5302: Day=Fri2, Slot=0, Hall=LR1, Students=75, Dept=ME</t>
+  </si>
+  <si>
+    <t>ME5303: Day=Fri, Slot=1, Hall=LT1, Students=75, Dept=ME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ME5204: Day=Sat, Slot=1, Hall=Civil-CSR, Students=75, Dept=ME      </t>
+  </si>
+  <si>
+    <t>ME5305: Day=Sun, Slot=1, Hall=New Computer Center, Students=75, Dept=ME</t>
+  </si>
+  <si>
+    <t>ME5210: Day=Wed, Slot=1, Hall=I.S. Seminar Room, Students=75, Dept=ME</t>
+  </si>
+  <si>
+    <t>ME5212: Day=Thu2, Slot=0, Hall=I.S. Seminar Room, Students=75, Dept=ME</t>
+  </si>
+  <si>
+    <t>ME5213: Day=Tue2, Slot=1, Hall=Electrical-ECC, Students=75, Dept=ME</t>
+  </si>
+  <si>
+    <t>IS5101: Day=Sat, Slot=1, Hall=AUD, Students=550, Dept=IS</t>
+  </si>
+  <si>
+    <t>IS5302: Day=Mon2, Slot=0, Hall=AUD, Students=550, Dept=IS</t>
+  </si>
+  <si>
+    <t>IS5303: Day=Sun, Slot=0, Hall=AUD, Students=550, Dept=IS</t>
+  </si>
+  <si>
+    <t>IS5306: Day=Sun, Slot=1, Hall=AUD, Students=550, Dept=IS</t>
+  </si>
+  <si>
+    <t>CE8301: Day=Mon, Slot=0, Hall=I.S. Seminar Room, Students=100, Dept=CE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CE7252: Day=Sat, Slot=1, Hall=Civil-COBEU, Students=100, Dept=CE   </t>
+  </si>
+  <si>
+    <t>CE7401: Day=Wed2, Slot=1, Hall=Old Computer Centre, Students=100, Dept=CE</t>
+  </si>
+  <si>
+    <t>CE7606: Day=Tue, Slot=0, Hall=NLH1, Students=100, Dept=CE</t>
+  </si>
+  <si>
+    <t>CE7205: Day=Sat, Slot=0, Hall=Old Computer Centre, Students=100, Dept=CE</t>
+  </si>
+  <si>
+    <t>EE7208: Day=Mon2, Slot=0, Hall=LR2, Students=75, Dept=EE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EE7802: Day=Wed, Slot=1, Hall=Civil-CSR, Students=75, Dept=EE      </t>
+  </si>
+  <si>
+    <t>EE8203: Day=Thu2, Slot=1, Hall=LT2, Students=75, Dept=EE</t>
+  </si>
+  <si>
+    <t>EE8204: Day=Mon2, Slot=1, Hall=Electrical-ECC, Students=75, Dept=EE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EE8206: Day=Tue, Slot=1, Hall=Mechanical-MLR, Students=75, Dept=EE </t>
+  </si>
+  <si>
+    <t>EE8208: Day=Sun2, Slot=0, Hall=Electrical-ESR, Students=75, Dept=EE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EE8210: Day=Sun, Slot=1, Hall=Electrical-ESR, Students=75, Dept=EE </t>
+  </si>
+  <si>
+    <t>EE8211: Day=Mon, Slot=1, Hall=AUD, Students=75, Dept=EE</t>
+  </si>
+  <si>
+    <t>EE8217: Day=Sat, Slot=1, Hall=LR1, Students=75, Dept=EE</t>
+  </si>
+  <si>
+    <t>EC7802: Day=Wed2, Slot=0, Hall=New Computer Center, Students=200, Dept=EC</t>
+  </si>
+  <si>
+    <t>EC8204: Day=Mon2, Slot=0, Hall=LT2, Students=200, Dept=EC</t>
+  </si>
+  <si>
+    <t>EC8205: Day=Fri2, Slot=0, Hall=New Computer Center, Students=200, Dept=EC</t>
+  </si>
+  <si>
+    <t>EC8206: Day=Mon, Slot=1, Hall=LT1, Students=200, Dept=EC</t>
+  </si>
+  <si>
+    <t>EC8207: Day=Tue, Slot=0, Hall=LT2, Students=200, Dept=EC</t>
+  </si>
+  <si>
+    <t>EC8208: Day=Thu, Slot=1, Hall=New Computer Center, Students=200, Dept=EC</t>
+  </si>
+  <si>
+    <t>ME8301: Day=Fri, Slot=0, Hall=LR2, Students=75, Dept=ME</t>
+  </si>
+  <si>
+    <t>ME8202: Day=Thu2, Slot=1, Hall=DO1, Students=75, Dept=ME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ME8211: Day=Tue, Slot=1, Hall=Electrical-ECC, Students=75, Dept=ME </t>
+  </si>
+  <si>
+    <t>ME8212: Day=Sat2, Slot=1, Hall=Mechanical-MLR, Students=75, Dept=ME</t>
+  </si>
+  <si>
+    <t>ME7401: Day=Fri2, Slot=1, Hall=I.S. Seminar Room, Students=75, Dept=ME</t>
+  </si>
+  <si>
+    <t>ME7604: Day=Sun2, Slot=1, Hall=AUD, Students=75, Dept=ME</t>
+  </si>
+  <si>
+    <t>IS8201: Day=Mon, Slot=0, Hall=AUD, Students=550, Dept=IS</t>
+  </si>
+  <si>
+    <t>GYM</t>
+  </si>
+  <si>
+    <t>Gym</t>
   </si>
 </sst>
 </file>
@@ -7871,6 +8179,289 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="7" max="7" width="23" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>589</v>
+      </c>
+      <c r="B1" t="s">
+        <v>590</v>
+      </c>
+      <c r="C1" t="s">
+        <v>591</v>
+      </c>
+      <c r="D1" t="s">
+        <v>592</v>
+      </c>
+      <c r="E1" t="s">
+        <v>593</v>
+      </c>
+      <c r="F1" t="s">
+        <v>594</v>
+      </c>
+      <c r="G1" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="str">
+        <f>IF(MID(A2,3,1)=" ",LEFT(A2,2)&amp;MID(A2,4,LEN(A2)-3),A2)</f>
+        <v>CE1202</v>
+      </c>
+      <c r="D2" t="str">
+        <f>MID(C2,4,1)</f>
+        <v>2</v>
+      </c>
+      <c r="E2" t="b">
+        <f>IF(F2="IS",TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="F2" t="str">
+        <f>LEFT(C2,2)</f>
+        <v>CE</v>
+      </c>
+      <c r="G2">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C10" si="0">IF(MID(A3,3,1)=" ",LEFT(A3,2)&amp;MID(A3,4,LEN(A3)-3),A3)</f>
+        <v>CE1101</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D9" si="1">MID(C3,4,1)</f>
+        <v>1</v>
+      </c>
+      <c r="E3" t="b">
+        <f t="shared" ref="E3:E10" si="2">IF(F3="IS",TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F10" si="3">LEFT(C3,2)</f>
+        <v>CE</v>
+      </c>
+      <c r="G3">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>EE1301</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="E4" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="3"/>
+        <v>EE</v>
+      </c>
+      <c r="G4">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>EE1101</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E5" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="3"/>
+        <v>EE</v>
+      </c>
+      <c r="G5">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>ME1201</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E6" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="3"/>
+        <v>ME</v>
+      </c>
+      <c r="G6">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>ME1202</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E7" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="3"/>
+        <v>ME</v>
+      </c>
+      <c r="G7">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>IS1402</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="E8" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="3"/>
+        <v>IS</v>
+      </c>
+      <c r="G8">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>IS1301</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="E9" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="3"/>
+        <v>IS</v>
+      </c>
+      <c r="G9">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>IS1003</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10" t="b">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="3"/>
+        <v>IS</v>
+      </c>
+      <c r="G10">
+        <v>550</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G100"/>
   <sheetViews>
     <sheetView topLeftCell="A91" workbookViewId="0">
@@ -10788,7 +11379,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B248"/>
   <sheetViews>
@@ -12791,12 +13382,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13445,6 +14036,469 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="34.140625" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" customWidth="1"/>
+    <col min="7" max="7" width="31" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>594</v>
+      </c>
+      <c r="B1" t="s">
+        <v>596</v>
+      </c>
+      <c r="C1" t="s">
+        <v>597</v>
+      </c>
+      <c r="D1" t="s">
+        <v>598</v>
+      </c>
+      <c r="E1" t="s">
+        <v>599</v>
+      </c>
+      <c r="F1" t="s">
+        <v>600</v>
+      </c>
+      <c r="G1" t="s">
+        <v>601</v>
+      </c>
+      <c r="H1" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>631</v>
+      </c>
+      <c r="B2">
+        <v>16</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>173</v>
+      </c>
+      <c r="F2" t="s">
+        <v>173</v>
+      </c>
+      <c r="G2" t="s">
+        <v>602</v>
+      </c>
+      <c r="H2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>631</v>
+      </c>
+      <c r="B3">
+        <v>17</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G3" t="s">
+        <v>603</v>
+      </c>
+      <c r="H3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>631</v>
+      </c>
+      <c r="B4">
+        <v>18</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F4" t="s">
+        <v>110</v>
+      </c>
+      <c r="G4" t="s">
+        <v>604</v>
+      </c>
+      <c r="H4">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>631</v>
+      </c>
+      <c r="B5">
+        <v>19</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" t="s">
+        <v>605</v>
+      </c>
+      <c r="H5">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>631</v>
+      </c>
+      <c r="B6">
+        <v>22</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>276</v>
+      </c>
+      <c r="F6" t="s">
+        <v>276</v>
+      </c>
+      <c r="G6" t="s">
+        <v>606</v>
+      </c>
+      <c r="H6">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>631</v>
+      </c>
+      <c r="B7">
+        <v>23</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>99</v>
+      </c>
+      <c r="F7" t="s">
+        <v>99</v>
+      </c>
+      <c r="G7" t="s">
+        <v>607</v>
+      </c>
+      <c r="H7">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>631</v>
+      </c>
+      <c r="B8">
+        <v>24</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>251</v>
+      </c>
+      <c r="F8" t="s">
+        <v>251</v>
+      </c>
+      <c r="G8" t="s">
+        <v>608</v>
+      </c>
+      <c r="H8">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>631</v>
+      </c>
+      <c r="B9">
+        <v>25</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>100</v>
+      </c>
+      <c r="F9" t="s">
+        <v>100</v>
+      </c>
+      <c r="G9" t="s">
+        <v>609</v>
+      </c>
+      <c r="H9">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>631</v>
+      </c>
+      <c r="B10">
+        <v>47</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1423</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1423</v>
+      </c>
+      <c r="G10" t="s">
+        <v>1424</v>
+      </c>
+      <c r="H10">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>631</v>
+      </c>
+      <c r="B11">
+        <v>27</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>612</v>
+      </c>
+      <c r="F11" t="s">
+        <v>613</v>
+      </c>
+      <c r="G11" t="s">
+        <v>614</v>
+      </c>
+      <c r="H11">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>631</v>
+      </c>
+      <c r="B12">
+        <v>28</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>321</v>
+      </c>
+      <c r="F12" t="s">
+        <v>321</v>
+      </c>
+      <c r="G12" t="s">
+        <v>615</v>
+      </c>
+      <c r="H12">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>631</v>
+      </c>
+      <c r="B13">
+        <v>29</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>616</v>
+      </c>
+      <c r="F13" t="s">
+        <v>271</v>
+      </c>
+      <c r="G13" t="s">
+        <v>617</v>
+      </c>
+      <c r="H13">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>631</v>
+      </c>
+      <c r="B14">
+        <v>30</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>618</v>
+      </c>
+      <c r="F14" t="s">
+        <v>618</v>
+      </c>
+      <c r="G14" t="s">
+        <v>618</v>
+      </c>
+      <c r="H14">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
+        <v>631</v>
+      </c>
+      <c r="B15">
+        <v>44</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>625</v>
+      </c>
+      <c r="F15" t="s">
+        <v>625</v>
+      </c>
+      <c r="G15" t="s">
+        <v>626</v>
+      </c>
+      <c r="H15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>631</v>
+      </c>
+      <c r="B16">
+        <v>45</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>627</v>
+      </c>
+      <c r="F16" t="s">
+        <v>627</v>
+      </c>
+      <c r="G16" t="s">
+        <v>628</v>
+      </c>
+      <c r="H16">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>631</v>
+      </c>
+      <c r="B17">
+        <v>46</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>629</v>
+      </c>
+      <c r="F17" t="s">
+        <v>629</v>
+      </c>
+      <c r="G17" t="s">
+        <v>630</v>
+      </c>
+      <c r="H17">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -39847,7 +40901,7 @@
   <dimension ref="A1:L362"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11:D36"/>
+      <selection activeCell="E2" sqref="E2:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -39902,8 +40956,7 @@
         <v>2</v>
       </c>
       <c r="E2" t="b">
-        <f>IF(F2="IS",TRUE,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" t="str">
         <f>LEFT(C2,2)</f>
@@ -39929,11 +40982,10 @@
         <v>1</v>
       </c>
       <c r="E3" t="b">
-        <f t="shared" ref="E3:E66" si="2">IF(F3="IS",TRUE,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F66" si="3">LEFT(C3,2)</f>
+        <f t="shared" ref="F3:F66" si="2">LEFT(C3,2)</f>
         <v>CE</v>
       </c>
       <c r="G3">
@@ -39956,11 +41008,10 @@
         <v>3</v>
       </c>
       <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F4" t="str">
-        <f t="shared" si="3"/>
         <v>EE</v>
       </c>
       <c r="G4">
@@ -39983,11 +41034,10 @@
         <v>1</v>
       </c>
       <c r="E5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F5" t="str">
-        <f t="shared" si="3"/>
         <v>EE</v>
       </c>
       <c r="G5">
@@ -40010,11 +41060,10 @@
         <v>2</v>
       </c>
       <c r="E6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F6" t="str">
-        <f t="shared" si="3"/>
         <v>ME</v>
       </c>
       <c r="G6">
@@ -40037,11 +41086,10 @@
         <v>2</v>
       </c>
       <c r="E7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F7" t="str">
-        <f t="shared" si="3"/>
         <v>ME</v>
       </c>
       <c r="G7">
@@ -40064,11 +41112,11 @@
         <v>4</v>
       </c>
       <c r="E8" t="b">
+        <f t="shared" ref="E2:E66" si="3">IF(F8="IS",TRUE,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="F8" t="str">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F8" t="str">
-        <f t="shared" si="3"/>
         <v>IS</v>
       </c>
       <c r="G8">
@@ -40091,11 +41139,11 @@
         <v>3</v>
       </c>
       <c r="E9" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="F9" t="str">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F9" t="str">
-        <f t="shared" si="3"/>
         <v>IS</v>
       </c>
       <c r="G9">
@@ -40117,11 +41165,11 @@
         <v>2</v>
       </c>
       <c r="E10" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="F10" t="str">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F10" t="str">
-        <f t="shared" si="3"/>
         <v>IS</v>
       </c>
       <c r="G10">
@@ -40144,11 +41192,11 @@
         <v>2</v>
       </c>
       <c r="E11" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F11" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F11" t="str">
-        <f t="shared" si="3"/>
         <v>CE</v>
       </c>
       <c r="G11">
@@ -40171,11 +41219,11 @@
         <v>2</v>
       </c>
       <c r="E12" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F12" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F12" t="str">
-        <f t="shared" si="3"/>
         <v>CE</v>
       </c>
       <c r="G12">
@@ -40198,11 +41246,11 @@
         <v>3</v>
       </c>
       <c r="E13" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F13" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F13" t="str">
-        <f t="shared" si="3"/>
         <v>CE</v>
       </c>
       <c r="G13">
@@ -40225,11 +41273,11 @@
         <v>3</v>
       </c>
       <c r="E14" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F14" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F14" t="str">
-        <f t="shared" si="3"/>
         <v>CE</v>
       </c>
       <c r="G14">
@@ -40252,11 +41300,11 @@
         <v>2</v>
       </c>
       <c r="E15" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F15" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F15" t="str">
-        <f t="shared" si="3"/>
         <v>CE</v>
       </c>
       <c r="G15">
@@ -40279,11 +41327,11 @@
         <v>3</v>
       </c>
       <c r="E16" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F16" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F16" t="str">
-        <f t="shared" si="3"/>
         <v>EE</v>
       </c>
       <c r="G16">
@@ -40306,11 +41354,11 @@
         <v>2</v>
       </c>
       <c r="E17" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F17" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F17" t="str">
-        <f t="shared" si="3"/>
         <v>EE</v>
       </c>
       <c r="G17">
@@ -40333,11 +41381,11 @@
         <v>2</v>
       </c>
       <c r="E18" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F18" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F18" t="str">
-        <f t="shared" si="3"/>
         <v>EE</v>
       </c>
       <c r="G18">
@@ -40360,11 +41408,11 @@
         <v>3</v>
       </c>
       <c r="E19" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F19" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F19" t="str">
-        <f t="shared" si="3"/>
         <v>EE</v>
       </c>
       <c r="G19">
@@ -40387,11 +41435,11 @@
         <v>2</v>
       </c>
       <c r="E20" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F20" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F20" t="str">
-        <f t="shared" si="3"/>
         <v>EE</v>
       </c>
       <c r="G20">
@@ -40414,11 +41462,11 @@
         <v>3</v>
       </c>
       <c r="E21" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F21" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F21" t="str">
-        <f t="shared" si="3"/>
         <v>EE</v>
       </c>
       <c r="G21">
@@ -40441,11 +41489,11 @@
         <v>3</v>
       </c>
       <c r="E22" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F22" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F22" t="str">
-        <f t="shared" si="3"/>
         <v>EC</v>
       </c>
       <c r="G22">
@@ -40468,11 +41516,11 @@
         <v>2</v>
       </c>
       <c r="E23" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F23" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F23" t="str">
-        <f t="shared" si="3"/>
         <v>EC</v>
       </c>
       <c r="G23">
@@ -40495,11 +41543,11 @@
         <v>2</v>
       </c>
       <c r="E24" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F24" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F24" t="str">
-        <f t="shared" si="3"/>
         <v>EC</v>
       </c>
       <c r="G24">
@@ -40522,11 +41570,11 @@
         <v>4</v>
       </c>
       <c r="E25" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F25" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F25" t="str">
-        <f t="shared" si="3"/>
         <v>EC</v>
       </c>
       <c r="G25">
@@ -40549,11 +41597,11 @@
         <v>3</v>
       </c>
       <c r="E26" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F26" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F26" t="str">
-        <f t="shared" si="3"/>
         <v>EC</v>
       </c>
       <c r="G26">
@@ -40576,11 +41624,11 @@
         <v>3</v>
       </c>
       <c r="E27" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F27" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F27" t="str">
-        <f t="shared" si="3"/>
         <v>ME</v>
       </c>
       <c r="G27">
@@ -40603,11 +41651,11 @@
         <v>2</v>
       </c>
       <c r="E28" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F28" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F28" t="str">
-        <f t="shared" si="3"/>
         <v>ME</v>
       </c>
       <c r="G28">
@@ -40630,11 +41678,11 @@
         <v>3</v>
       </c>
       <c r="E29" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F29" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F29" t="str">
-        <f t="shared" si="3"/>
         <v>ME</v>
       </c>
       <c r="G29">
@@ -40657,11 +41705,11 @@
         <v>2</v>
       </c>
       <c r="E30" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F30" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F30" t="str">
-        <f t="shared" si="3"/>
         <v>ME</v>
       </c>
       <c r="G30">
@@ -40684,7 +41732,7 @@
         <v>3</v>
       </c>
       <c r="E31" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F31" t="str">
@@ -40711,11 +41759,11 @@
         <v>2</v>
       </c>
       <c r="E32" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F32" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F32" t="str">
-        <f t="shared" si="3"/>
         <v>ME</v>
       </c>
       <c r="G32">
@@ -40738,11 +41786,11 @@
         <v>2</v>
       </c>
       <c r="E33" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F33" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F33" t="str">
-        <f t="shared" si="3"/>
         <v>ME</v>
       </c>
       <c r="G33">
@@ -40765,11 +41813,11 @@
         <v>3</v>
       </c>
       <c r="E34" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="F34" t="str">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F34" t="str">
-        <f t="shared" si="3"/>
         <v>IS</v>
       </c>
       <c r="G34">
@@ -40792,11 +41840,11 @@
         <v>3</v>
       </c>
       <c r="E35" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="F35" t="str">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F35" t="str">
-        <f t="shared" si="3"/>
         <v>IS</v>
       </c>
       <c r="G35">
@@ -40819,11 +41867,11 @@
         <v>3</v>
       </c>
       <c r="E36" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="F36" t="str">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F36" t="str">
-        <f t="shared" si="3"/>
         <v>IS</v>
       </c>
       <c r="G36">
@@ -40846,11 +41894,11 @@
         <v>3</v>
       </c>
       <c r="E37" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F37" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F37" t="str">
-        <f t="shared" si="3"/>
         <v>CE</v>
       </c>
       <c r="G37">
@@ -40873,11 +41921,11 @@
         <v>2</v>
       </c>
       <c r="E38" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F38" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F38" t="str">
-        <f t="shared" si="3"/>
         <v>CE</v>
       </c>
       <c r="G38">
@@ -40900,11 +41948,11 @@
         <v>3</v>
       </c>
       <c r="E39" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F39" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F39" t="str">
-        <f t="shared" si="3"/>
         <v>CE</v>
       </c>
       <c r="G39">
@@ -40927,11 +41975,11 @@
         <v>2</v>
       </c>
       <c r="E40" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F40" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F40" t="str">
-        <f t="shared" si="3"/>
         <v>CE</v>
       </c>
       <c r="G40">
@@ -40954,11 +42002,11 @@
         <v>2</v>
       </c>
       <c r="E41" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F41" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F41" t="str">
-        <f t="shared" si="3"/>
         <v>CE</v>
       </c>
       <c r="G41">
@@ -40981,11 +42029,11 @@
         <v>3</v>
       </c>
       <c r="E42" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F42" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F42" t="str">
-        <f t="shared" si="3"/>
         <v>CE</v>
       </c>
       <c r="G42">
@@ -41008,11 +42056,11 @@
         <v>2</v>
       </c>
       <c r="E43" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F43" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F43" t="str">
-        <f t="shared" si="3"/>
         <v>CE</v>
       </c>
       <c r="G43">
@@ -41035,11 +42083,11 @@
         <v>2</v>
       </c>
       <c r="E44" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F44" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F44" t="str">
-        <f t="shared" si="3"/>
         <v>CE</v>
       </c>
       <c r="G44">
@@ -41066,7 +42114,7 @@
         <v>0</v>
       </c>
       <c r="F45" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>EE</v>
       </c>
       <c r="G45">
@@ -41089,11 +42137,11 @@
         <v>3</v>
       </c>
       <c r="E46" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F46" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F46" t="str">
-        <f t="shared" si="3"/>
         <v>EE</v>
       </c>
       <c r="G46">
@@ -41116,11 +42164,11 @@
         <v>3</v>
       </c>
       <c r="E47" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F47" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F47" t="str">
-        <f t="shared" si="3"/>
         <v>EE</v>
       </c>
       <c r="G47">
@@ -41143,11 +42191,11 @@
         <v>3</v>
       </c>
       <c r="E48" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F48" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F48" t="str">
-        <f t="shared" si="3"/>
         <v>EE</v>
       </c>
       <c r="G48">
@@ -41170,11 +42218,11 @@
         <v>3</v>
       </c>
       <c r="E49" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F49" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F49" t="str">
-        <f t="shared" si="3"/>
         <v>EE</v>
       </c>
       <c r="G49">
@@ -41197,11 +42245,11 @@
         <v>2</v>
       </c>
       <c r="E50" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F50" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F50" t="str">
-        <f t="shared" si="3"/>
         <v>EE</v>
       </c>
       <c r="G50">
@@ -41224,11 +42272,11 @@
         <v>2</v>
       </c>
       <c r="E51" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F51" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F51" t="str">
-        <f t="shared" si="3"/>
         <v>EE</v>
       </c>
       <c r="G51">
@@ -41251,11 +42299,11 @@
         <v>2</v>
       </c>
       <c r="E52" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F52" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F52" t="str">
-        <f t="shared" si="3"/>
         <v>EE</v>
       </c>
       <c r="G52">
@@ -41278,11 +42326,11 @@
         <v>2</v>
       </c>
       <c r="E53" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F53" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F53" t="str">
-        <f t="shared" si="3"/>
         <v>EE</v>
       </c>
       <c r="G53">
@@ -41305,11 +42353,11 @@
         <v>4</v>
       </c>
       <c r="E54" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F54" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F54" t="str">
-        <f t="shared" si="3"/>
         <v>EE</v>
       </c>
       <c r="G54">
@@ -41332,7 +42380,7 @@
         <v>2</v>
       </c>
       <c r="E55" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F55" t="str">
@@ -41359,11 +42407,11 @@
         <v>3</v>
       </c>
       <c r="E56" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F56" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F56" t="str">
-        <f t="shared" si="3"/>
         <v>EE</v>
       </c>
       <c r="G56">
@@ -41386,11 +42434,11 @@
         <v>2</v>
       </c>
       <c r="E57" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F57" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F57" t="str">
-        <f t="shared" si="3"/>
         <v>EE</v>
       </c>
       <c r="G57">
@@ -41413,11 +42461,11 @@
         <v>4</v>
       </c>
       <c r="E58" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F58" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F58" t="str">
-        <f t="shared" si="3"/>
         <v>EE</v>
       </c>
       <c r="G58">
@@ -41440,11 +42488,11 @@
         <v>3</v>
       </c>
       <c r="E59" t="b">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="F59" t="str">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F59" t="str">
-        <f t="shared" si="3"/>
         <v>IS</v>
       </c>
       <c r="G59">
@@ -41467,11 +42515,11 @@
         <v>2</v>
       </c>
       <c r="E60" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F60" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F60" t="str">
-        <f t="shared" si="3"/>
         <v>EE</v>
       </c>
       <c r="G60">
@@ -41494,11 +42542,11 @@
         <v>2</v>
       </c>
       <c r="E61" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F61" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F61" t="str">
-        <f t="shared" si="3"/>
         <v>EE</v>
       </c>
       <c r="G61">
@@ -41521,11 +42569,11 @@
         <v>2</v>
       </c>
       <c r="E62" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F62" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F62" t="str">
-        <f t="shared" si="3"/>
         <v>EE</v>
       </c>
       <c r="G62">
@@ -41548,11 +42596,11 @@
         <v>3</v>
       </c>
       <c r="E63" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F63" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F63" t="str">
-        <f t="shared" si="3"/>
         <v>ME</v>
       </c>
       <c r="G63">
@@ -41575,11 +42623,11 @@
         <v>3</v>
       </c>
       <c r="E64" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F64" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F64" t="str">
-        <f t="shared" si="3"/>
         <v>ME</v>
       </c>
       <c r="G64">
@@ -41602,11 +42650,11 @@
         <v>3</v>
       </c>
       <c r="E65" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F65" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F65" t="str">
-        <f t="shared" si="3"/>
         <v>ME</v>
       </c>
       <c r="G65">
@@ -41629,11 +42677,11 @@
         <v>2</v>
       </c>
       <c r="E66" t="b">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F66" t="str">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F66" t="str">
-        <f t="shared" si="3"/>
         <v>ME</v>
       </c>
       <c r="G66">
@@ -41652,7 +42700,7 @@
         <v>ME5305</v>
       </c>
       <c r="D67">
-        <f t="shared" ref="D67:D80" si="5">VALUE(MID(C67,4,1))</f>
+        <f t="shared" ref="D67:D77" si="5">VALUE(MID(C67,4,1))</f>
         <v>3</v>
       </c>
       <c r="E67" t="b">
@@ -42614,6 +43662,522 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:A101"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="86.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>1324</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>1325</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>1326</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>1327</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>1330</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>1331</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>1332</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>1333</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>1334</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>1335</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>1336</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>1337</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>1338</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>1339</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>1340</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>1341</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>1342</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>1343</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>1344</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>1345</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>1346</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>1347</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>1348</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>1349</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>1351</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>1352</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>1353</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>1355</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>1356</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>1357</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>1358</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>1359</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>1361</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>1363</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" t="s">
+        <v>1364</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>1365</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>1366</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>1367</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" t="s">
+        <v>1368</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" t="s">
+        <v>1369</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>1370</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" t="s">
+        <v>1372</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" t="s">
+        <v>1373</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" t="s">
+        <v>1374</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" t="s">
+        <v>1375</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" t="s">
+        <v>1376</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" t="s">
+        <v>1377</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" t="s">
+        <v>1378</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" t="s">
+        <v>1379</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" t="s">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" t="s">
+        <v>1381</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" t="s">
+        <v>1384</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" t="s">
+        <v>1385</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" t="s">
+        <v>1386</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" t="s">
+        <v>1387</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" t="s">
+        <v>1388</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" t="s">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" t="s">
+        <v>1391</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" t="s">
+        <v>1393</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" t="s">
+        <v>1394</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" t="s">
+        <v>1395</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" t="s">
+        <v>1396</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" t="s">
+        <v>1397</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" t="s">
+        <v>1398</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" t="s">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" t="s">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" t="s">
+        <v>1402</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" t="s">
+        <v>1404</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" t="s">
+        <v>1405</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" t="s">
+        <v>1406</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" t="s">
+        <v>1407</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" t="s">
+        <v>1408</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" t="s">
+        <v>1409</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" t="s">
+        <v>1411</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" t="s">
+        <v>1412</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" t="s">
+        <v>1414</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" t="s">
+        <v>1415</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95" t="s">
+        <v>1416</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" t="s">
+        <v>1417</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" t="s">
+        <v>1418</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" t="s">
+        <v>1419</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" t="s">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" t="s">
+        <v>1421</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" t="s">
+        <v>1422</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A248"/>
   <sheetViews>
@@ -43871,7 +45435,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A102"/>
   <sheetViews>
@@ -44397,287 +45961,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="7" max="7" width="23" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
-        <v>589</v>
-      </c>
-      <c r="B1" t="s">
-        <v>590</v>
-      </c>
-      <c r="C1" t="s">
-        <v>591</v>
-      </c>
-      <c r="D1" t="s">
-        <v>592</v>
-      </c>
-      <c r="E1" t="s">
-        <v>593</v>
-      </c>
-      <c r="F1" t="s">
-        <v>594</v>
-      </c>
-      <c r="G1" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="str">
-        <f>IF(MID(A2,3,1)=" ",LEFT(A2,2)&amp;MID(A2,4,LEN(A2)-3),A2)</f>
-        <v>CE1202</v>
-      </c>
-      <c r="D2" t="str">
-        <f>MID(C2,4,1)</f>
-        <v>2</v>
-      </c>
-      <c r="E2" t="b">
-        <f>IF(F2="IS",TRUE,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="F2" t="str">
-        <f>LEFT(C2,2)</f>
-        <v>CE</v>
-      </c>
-      <c r="G2">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="str">
-        <f t="shared" ref="C3:C10" si="0">IF(MID(A3,3,1)=" ",LEFT(A3,2)&amp;MID(A3,4,LEN(A3)-3),A3)</f>
-        <v>CE1101</v>
-      </c>
-      <c r="D3" t="str">
-        <f t="shared" ref="D3:D9" si="1">MID(C3,4,1)</f>
-        <v>1</v>
-      </c>
-      <c r="E3" t="b">
-        <f t="shared" ref="E3:E10" si="2">IF(F3="IS",TRUE,FALSE)</f>
-        <v>0</v>
-      </c>
-      <c r="F3" t="str">
-        <f t="shared" ref="F3:F10" si="3">LEFT(C3,2)</f>
-        <v>CE</v>
-      </c>
-      <c r="G3">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="str">
-        <f t="shared" si="0"/>
-        <v>EE1301</v>
-      </c>
-      <c r="D4" t="str">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="E4" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F4" t="str">
-        <f t="shared" si="3"/>
-        <v>EE</v>
-      </c>
-      <c r="G4">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" t="str">
-        <f t="shared" si="0"/>
-        <v>EE1101</v>
-      </c>
-      <c r="D5" t="str">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E5" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F5" t="str">
-        <f t="shared" si="3"/>
-        <v>EE</v>
-      </c>
-      <c r="G5">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="str">
-        <f t="shared" si="0"/>
-        <v>ME1201</v>
-      </c>
-      <c r="D6" t="str">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="E6" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F6" t="str">
-        <f t="shared" si="3"/>
-        <v>ME</v>
-      </c>
-      <c r="G6">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7" t="str">
-        <f t="shared" si="0"/>
-        <v>ME1202</v>
-      </c>
-      <c r="D7" t="str">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="E7" t="b">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F7" t="str">
-        <f t="shared" si="3"/>
-        <v>ME</v>
-      </c>
-      <c r="G7">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8" t="str">
-        <f t="shared" si="0"/>
-        <v>IS1402</v>
-      </c>
-      <c r="D8" t="str">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="E8" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F8" t="str">
-        <f t="shared" si="3"/>
-        <v>IS</v>
-      </c>
-      <c r="G8">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9" t="str">
-        <f t="shared" si="0"/>
-        <v>IS1301</v>
-      </c>
-      <c r="D9" t="str">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="E9" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F9" t="str">
-        <f t="shared" si="3"/>
-        <v>IS</v>
-      </c>
-      <c r="G9">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10" t="str">
-        <f t="shared" si="0"/>
-        <v>IS1003</v>
-      </c>
-      <c r="D10">
-        <v>2</v>
-      </c>
-      <c r="E10" t="b">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="F10" t="str">
-        <f t="shared" si="3"/>
-        <v>IS</v>
-      </c>
-      <c r="G10">
-        <v>550</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>